<commit_message>
fix: perbaikan dataset untuk kalimat yang tidak mengandung kolom
</commit_message>
<xml_diff>
--- a/detectors/whereopr/dataset/dataset.xlsx
+++ b/detectors/whereopr/dataset/dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pras\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\codes\nl2sql\detectors\whereopr\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3067537C-BB83-4A32-91F4-AC80E2036735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE27EB82-E832-40C4-BDA8-D7A2A23A5C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17528,7 +17528,7 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -17705,7 +17705,7 @@
     </row>
     <row r="7" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>0</v>
+        <v>582</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>265</v>
@@ -17740,7 +17740,7 @@
     </row>
     <row r="8" spans="1:25" s="19" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
-        <v>0</v>
+        <v>582</v>
       </c>
       <c r="B8" s="28" t="s">
         <v>266</v>

</xml_diff>